<commit_message>
k1 and k5 series making standard CPA
</commit_message>
<xml_diff>
--- a/static/finalOutput/listOfQty.xlsx
+++ b/static/finalOutput/listOfQty.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
   <si>
     <t>PART NO.</t>
   </si>
@@ -58,7 +58,7 @@
     <t>F9300AF</t>
   </si>
   <si>
-    <t>F9900GD</t>
+    <t>F9900GE</t>
   </si>
   <si>
     <t>F9900RJ</t>
@@ -79,15 +79,24 @@
     <t>F9342MK</t>
   </si>
   <si>
-    <t>F9340SB</t>
-  </si>
-  <si>
-    <t>D0114PB</t>
+    <t>F9900TB</t>
+  </si>
+  <si>
+    <t>F9900EA</t>
+  </si>
+  <si>
+    <t>F9275ED</t>
   </si>
   <si>
     <t>D0114RZ</t>
   </si>
   <si>
+    <t>F9900AC</t>
+  </si>
+  <si>
+    <t>F9900BC</t>
+  </si>
+  <si>
     <t>F9300TE</t>
   </si>
   <si>
@@ -130,6 +139,27 @@
     <t>G9330DB</t>
   </si>
   <si>
+    <t>F9275ZZ</t>
+  </si>
+  <si>
+    <t>F9340ND</t>
+  </si>
+  <si>
+    <t>C1016EZ</t>
+  </si>
+  <si>
+    <t>F9203ZA</t>
+  </si>
+  <si>
+    <t>F9275EF</t>
+  </si>
+  <si>
+    <t>F9275EG</t>
+  </si>
+  <si>
+    <t>Y9400ET</t>
+  </si>
+  <si>
     <t>F9341JD</t>
   </si>
   <si>
@@ -142,7 +172,25 @@
     <t>F9341JA</t>
   </si>
   <si>
-    <t>CPA110Y-NFS5G-9NNNN/MG1</t>
+    <t>CPA110Y-NVSNN-NNNNN</t>
+  </si>
+  <si>
+    <t>F9940WF</t>
+  </si>
+  <si>
+    <t>F9900SF</t>
+  </si>
+  <si>
+    <t>F9900SN</t>
+  </si>
+  <si>
+    <t>F9900SK</t>
+  </si>
+  <si>
+    <t>F9900MK</t>
+  </si>
+  <si>
+    <t>CPA530Y-NCS4N-0NNNN</t>
   </si>
   <si>
     <t>TERMINAL COVER</t>
@@ -187,12 +235,15 @@
     <t>NUT</t>
   </si>
   <si>
+    <t>FLANGE</t>
+  </si>
+  <si>
+    <t>GASCKET</t>
+  </si>
+  <si>
     <t>VENT PLUG</t>
   </si>
   <si>
-    <t>VENT SCREW</t>
-  </si>
-  <si>
     <t>PLUG</t>
   </si>
   <si>
@@ -226,6 +277,15 @@
     <t>PLUG RED</t>
   </si>
   <si>
+    <t>LABEL</t>
+  </si>
+  <si>
+    <t>SOLID SUB-MATERIALS</t>
+  </si>
+  <si>
+    <t>NEEDLE ASSY</t>
+  </si>
+  <si>
     <t>Spring</t>
   </si>
   <si>
@@ -233,6 +293,9 @@
   </si>
   <si>
     <t>CPA</t>
+  </si>
+  <si>
+    <t>PIPE ASSY</t>
   </si>
 </sst>
 </file>
@@ -590,7 +653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -615,10 +678,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -629,10 +692,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -643,10 +706,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -657,10 +720,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -671,10 +734,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D6">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -685,10 +748,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -699,10 +762,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -713,10 +776,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D9">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -727,10 +790,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -741,10 +804,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -755,10 +818,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -769,10 +832,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -783,10 +846,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -797,10 +860,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -811,10 +874,10 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -825,10 +888,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -839,10 +902,10 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -853,10 +916,10 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D19">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -867,248 +930,248 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D20">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D22">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="D25">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D26">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D28">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D29">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D30">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D36">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1119,10 +1182,10 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1133,38 +1196,262 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="D39">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D40">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>88</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>89</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>90</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>91</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>93</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>100</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>